<commit_message>
new tests for fuincexec are added and new message format in test is used
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\spreadsheet_analytics\project\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22665" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="22665" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Constant Values</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Expected Values</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -391,18 +394,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
@@ -416,7 +419,7 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -440,7 +443,7 @@
         <f ca="1">FUNCEXEC("DEF_1", 1, 2)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>3</v>
       </c>
       <c r="D2" t="e">
@@ -466,7 +469,7 @@
         <f ca="1">FUNCEXEC("DEF_1", 2, 2)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>4</v>
       </c>
       <c r="E3" s="1"/>
@@ -479,7 +482,7 @@
         <f ca="1">FUNCEXEC("DEF_1", K2, 2)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>14</v>
       </c>
       <c r="K4">
@@ -491,7 +494,7 @@
         <f ca="1">FUNCEXEC("DEF_1", 2, K3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>5</v>
       </c>
     </row>
@@ -500,7 +503,7 @@
         <f ca="1">FUNCEXEC("DEF_1", K2, K3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>15</v>
       </c>
     </row>
@@ -509,7 +512,7 @@
         <f ca="1">FUNCEXEC("DEF_1", None, K3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C7" t="e">
+      <c r="B7" t="e">
         <f>SUM(None, K3)</f>
         <v>#NAME?</v>
       </c>
@@ -519,7 +522,7 @@
         <f ca="1">FUNCEXEC("DEF_1", "None", K3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>3</v>
       </c>
     </row>
@@ -528,7 +531,7 @@
         <f ca="1">FUNCEXEC("DEF_1", "Nodata", "Nodata")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
@@ -537,7 +540,7 @@
         <f ca="1">FUNCEXEC("DEF_1", K3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C10" t="e">
+      <c r="B10" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -546,8 +549,193 @@
         <f ca="1">FUNCEXEC("DEF_1", K2, K3, K4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C11" t="e">
+      <c r="B11" t="e">
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="e">
+        <f ca="1">FUNCEXEC("lowercase")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B12">
+        <v>42</v>
+      </c>
+      <c r="D12" t="e">
+        <f ca="1">DEFINE("lowercase","#",E12)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="e">
+        <f ca="1">FUNCEXEC("LOWERCASE")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="e">
+        <f ca="1">FUNCEXEC("LoWeRcAsE")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="e">
+        <f ca="1">FUNCEXEC("LoWeRcAsE",1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B15" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="e">
+        <f ca="1">FUNCEXEC("NoSuchDefine",1,2,3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B16" t="e">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="e">
+        <f ca="1">FUNCEXEC("OutEqualsIn",56)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B17">
+        <v>56</v>
+      </c>
+      <c r="D17" t="e">
+        <f ca="1">DEFINE("OutEqualsIn",E17,"#",E17)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="e">
+        <f ca="1">FUNCEXEC("OutEqualsIn",E18)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B18">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="e">
+        <f ca="1">FUNCEXEC("OutEqualsIn",E19)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B19">
+        <v>56</v>
+      </c>
+      <c r="E19">
+        <f>E18</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="e">
+        <f ca="1">FUNCEXEC("OutEqualsIn",E20)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="e">
+        <f ca="1">FUNCEXEC("OutEqualsIn",E21)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="str">
+        <f>E20</f>
+        <v>Text</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="e">
+        <f ca="1">FUNCEXEC("RangeInOut",K22:M22)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="e">
+        <f ca="1">DEFINE("RangeInOut",E22,F22,G22,"#",H22,I22,J22)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H22">
+        <f>E22+1</f>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f>F22+1</f>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f>G22+1</f>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="e">
+        <f ca="1">INDEX(FUNCEXEC("RangeInOut",K23:M23),1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="e">
+        <f ca="1">INDEX(FUNCEXEC("RangeInOut",K24:M24),2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="e">
+        <f ca="1">INDEX(FUNCEXEC("RangeInOut",K25:M25),3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="e">
+        <f ca="1">INDEX(FUNCEXEC("RangeInOut",K26:M26),10)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B26" t="e">
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEFINE function name toUpperCase is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="22665" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22665" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#96 another one test for FUNCEXEC
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-demo\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +774,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="e">
+        <f ca="1">FUNCEXEC("DEF_1", K27:L27)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Funcexec test (and functionality) is fixed
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Funcexec_Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\spreadsheet_analytics\project\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22665" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="22665" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,12 +509,11 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="e">
-        <f ca="1">FUNCEXEC("DEF_1", None, K3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="B7" t="e">
-        <f>SUM(None, K3)</f>
-        <v>#NAME?</v>
+        <f ca="1">FUNCEXEC("DEF_1", "None", K3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>